<commit_message>
add akka cluster demo
</commit_message>
<xml_diff>
--- a/reference/Q&A.xlsx
+++ b/reference/Q&A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23805" windowHeight="12090" activeTab="1"/>
+    <workbookView windowWidth="22155" windowHeight="11355"/>
   </bookViews>
   <sheets>
     <sheet name="知识面" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>备注1</t>
   </si>
@@ -97,7 +97,18 @@
 Patterns.ask 是使用一个临时创建的actor发消息而非自身</t>
   </si>
   <si>
-    <t>Akka Cluster not in use - Using Akka Cluster is recommended if you need remote watch and deploy</t>
+    <t>Akka Cluster not in use - Using Akka Cluster is recommended if you need remote watch and deploy
+Actor的最佳实践
+Actor尽量不要阻塞
+Actor间不要传递可变对象
+Actor的state， behavior作为可变对象，不要在actor间传递。
+Top-level actors尽量少创建
+actor会自动管理我们分配的固定资源。一个actor system可能有上百万个actors,毕竟actor是非常轻量级的，每个实例只占300字节</t>
+  </si>
+  <si>
+    <t>在微服务架构中，你应该考虑服务内部和服务之间的通信。
+https://blog.csdn.net/qq_35246620/article/details/78070474
+一般来说，我们建议不要在不同的服务之间使用 Akka 集群和 Actor 消息传递，因为这会导致服务之间的代码耦合过紧，并且难以独立地部署这些服务，这是使用微服务架构的主要原因之一。</t>
   </si>
   <si>
     <t>thingsboard全面讲解</t>
@@ -489,6 +500,13 @@
 Docker for Windows 有两种运行模式，一种运行Windows相关容器，一种运行传统的Linux容器。同一时间只能选择一种模式运行。</t>
   </si>
   <si>
+    <t>kafka</t>
+  </si>
+  <si>
+    <t>https://www.cnblogs.com/jackspan/p/11179787.html
+kafka 一个consumer可以订阅多个topic，且可以使用正则表达式。</t>
+  </si>
+  <si>
     <t>阳春白雪</t>
   </si>
   <si>
@@ -500,10 +518,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -523,14 +541,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -544,6 +600,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -552,21 +660,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -575,44 +668,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -621,43 +676,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -674,6 +692,96 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -686,7 +794,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,43 +830,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,115 +848,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,54 +897,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -957,6 +927,63 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -971,15 +998,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -988,145 +1006,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1499,8 +1517,8 @@
   <sheetPr/>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1594,7 +1612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" ht="100" customHeight="1" spans="1:4">
+    <row r="12" ht="100" customHeight="1" spans="1:5">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1604,96 +1622,99 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" ht="209.5" customHeight="1" spans="1:6">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" ht="54" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" ht="175.5" spans="1:3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" ht="67.5" spans="1:3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" ht="27" spans="1:4">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1706,10 +1727,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A15" sqref="$A15:$XFD15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1722,142 +1743,150 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" ht="100" customHeight="1" spans="1:2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" ht="100" customHeight="1" spans="1:6">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" ht="100" customHeight="1" spans="1:1">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" ht="100" customHeight="1" spans="1:3">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" ht="100" customHeight="1" spans="1:1">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" ht="100" customHeight="1" spans="1:1">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" ht="100" customHeight="1" spans="1:1">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" ht="100" customHeight="1" spans="1:2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" ht="100" customHeight="1" spans="1:6">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" ht="100" customHeight="1" spans="1:1">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" ht="100" customHeight="1" spans="1:2">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" ht="100" customHeight="1" spans="1:4">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" ht="100" customHeight="1" spans="1:3">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="5" t="s">
         <v>81</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" ht="67.5" spans="1:2">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1887,10 +1916,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add kafka producer and consumer
</commit_message>
<xml_diff>
--- a/reference/Q&A.xlsx
+++ b/reference/Q&A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22155" windowHeight="11355"/>
+    <workbookView windowWidth="18345" windowHeight="11355"/>
   </bookViews>
   <sheets>
     <sheet name="知识面" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>备注1</t>
   </si>
@@ -97,7 +97,11 @@
 Patterns.ask 是使用一个临时创建的actor发消息而非自身</t>
   </si>
   <si>
-    <t>Akka Cluster not in use - Using Akka Cluster is recommended if you need remote watch and deploy
+    <t>十分钟理解Actor:
+https://blog.51cto.com/nxlhero/1666250
+为什么说akka是高并发事务的真正终极解决方案:
+https://www.jdon.com/45728
+Akka Cluster not in use - Using Akka Cluster is recommended if you need remote watch and deploy
 Actor的最佳实践
 Actor尽量不要阻塞
 Actor间不要传递可变对象
@@ -109,6 +113,14 @@
     <t>在微服务架构中，你应该考虑服务内部和服务之间的通信。
 https://blog.csdn.net/qq_35246620/article/details/78070474
 一般来说，我们建议不要在不同的服务之间使用 Akka 集群和 Actor 消息传递，因为这会导致服务之间的代码耦合过紧，并且难以独立地部署这些服务，这是使用微服务架构的主要原因之一。</t>
+  </si>
+  <si>
+    <t>在不同的服务之间，「Akka HTTP」或「Akka gRPC」可用于同步（但不阻塞）通信，而「Akka Streams Kafka」或其他「Alpakka」连接器可用于集成异步通信。所有这些通信机制都可以很好地与端到端的反向压力（end-to-end back-pressure）的消息流配合使用，同步通信工具也可以用于单个请求-响应（request response）交互。同样重要的是要注意，当使用这些工具时，通信的双方不必使用 Akka 实现，编程语言也不重要。</t>
+  </si>
+  <si>
+    <t>2. 部分API已经过时，比如：
+官网Java示例重写receive方法中用的是receiveBuilder().match去进行匹配，书中还是if xxx instanceof xxx。
+官网Java示例Actor继承AbstractActor，书中用的是已经过时(2.5.0版本开始)的UntypedActor</t>
   </si>
   <si>
     <t>thingsboard全面讲解</t>
@@ -144,9 +156,9 @@
 npm install -g cnpm --registry=http://registry.npm.taobao.org</t>
   </si>
   <si>
-    <t xml:space="preserve">tb 2.4数据库表结构：
+    <t>tb 2.4数据库表结构：
 https://www.pianshen.com/article/4695822890/
-</t>
+tb rule engine各Actor的功能说明：https://www.iotschool.com/topics/46</t>
   </si>
   <si>
     <r>
@@ -191,6 +203,40 @@
     </r>
   </si>
   <si>
+    <r>
+      <t>下面列出了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>每个 actor 功能的简要说明</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+App Actor - 负责管理租户演员。此 actor 的示例始终存在于内存中。
+租户演员 - 负责管理租户设备和规则链演员。此 actor 的实例始终存在于内存中。
+Device Actor - 维护设备的状态:活动回话，订阅，挂起的 RPC 命令等。出于性能原因，将当前设备属性缓存在内存中。处理来自设备的第一条消息时，将创建一个 actor。当设备在一段时间内没有消息时，actor 停止。
+规则链 Actor - 处理传入的消息，将它们保存到队列中并将它们分派给规则节点 actor。此 actor 的实例始终存在于内存中。
+规则节点 Actor - 处理传入消息，并将结果报告给规则链 actor。此 actor 的实例始终存在于内存中。
+设备会话管理器 Actor - 负责管理设备会话 actor。在具有相应会话 ID 的第一条消息上创建会话 actor。关闭相应会话时关闭会话 actor。
+Session Actor - 表示设备和 ThingsBoard 服务器之间的通信会话。会话可以是同步的 (HTTP,COAP) 和异步的 (MQTT,带有 Observe 选项的 CoAP)。
+RPC 会话管理器 Actor - 负责管理集群 RPC 会话 actor。新服务器启动时创建会话 actor。服务器关闭时关闭会话 actor。
+RPC Session Actor - 表示集群模式下 2 个 ThingsBoard 服务器之间的通信会话。使用基于 gPRC 的 HTTP/2 进行通信。</t>
+    </r>
+  </si>
+  <si>
     <t>rule engine全面讲解</t>
   </si>
   <si>
@@ -250,7 +296,11 @@
   <si>
     <t>在开始使用SchedulerX前，需要先开通。SchedulerX目前在公测期，免费。
 背景信息
-分布式任务调度目前处于公测期，免费使用。</t>
+SchedulerX分布式任务调度目前处于公测期，免费使用。</t>
+  </si>
+  <si>
+    <t>重要的原理及源码分析文章（包含worker如何选主，server和worker的通信方式）：
+https://www.cnblogs.com/xueweihan/p/13477189.html</t>
   </si>
   <si>
     <t>常见的流媒体协议</t>
@@ -507,6 +557,32 @@
 kafka 一个consumer可以订阅多个topic，且可以使用正则表达式。</t>
   </si>
   <si>
+    <t>powerjob执行一次</t>
+  </si>
+  <si>
+    <t>我定义了一个固定时间的任务，为啥到那个时间后一直启动新的实例，不断的刷新执行任务，我怎样控制只让任务执行一次
+tjq07-30 14:42
+回复 @huyan回到原评论
+FixDelay/FixRate 统称秒级任务，秒级任务只有任务本身被关闭的情况下才会停止调度，否则即使你停止上一个任务实例，系统也会根据容错策略启动新的秒级任务实例。
+执行一次应该选择“API”定时类型，使用 OpenAPI 去触发任务。</t>
+  </si>
+  <si>
+    <t>docker和vmware冲突临时解决办法</t>
+  </si>
+  <si>
+    <t>Hyper-V与VMware是无法共存，装了docker-desktop ，vmware就不能用了
+使用vmware
+在cmd里运行     bcdedit /set hypervisorlaunchtype off      重启电脑
+使用docker-desktop
+在cmd里运行     bcdedit /set hypervisorlaunchtype auto     重启电脑</t>
+  </si>
+  <si>
+    <t>基于LMAX系统的交易所高并发低延迟系统架构解析与优化</t>
+  </si>
+  <si>
+    <t>https://wenku.baidu.com/view/cd72d264900ef12d2af90242a8956bec0875a5da.html</t>
+  </si>
+  <si>
     <t>阳春白雪</t>
   </si>
   <si>
@@ -518,10 +594,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -541,7 +617,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -555,22 +631,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,9 +652,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -609,54 +730,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -692,187 +768,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,8 +1006,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -939,8 +1030,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -960,30 +1051,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -998,6 +1065,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1006,10 +1082,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1018,16 +1094,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1036,119 +1112,119 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1165,6 +1241,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1515,19 +1594,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="E14" sqref="$A14:$XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="34.375" customWidth="1"/>
     <col min="2" max="2" width="35.5" customWidth="1"/>
     <col min="3" max="3" width="50.75" customWidth="1"/>
     <col min="4" max="4" width="72.25" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
+    <col min="7" max="7" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1612,7 +1692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" ht="100" customHeight="1" spans="1:5">
+    <row r="12" ht="100" customHeight="1" spans="1:7">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1622,99 +1702,111 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" ht="209.5" customHeight="1" spans="1:6">
+      <c r="F12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" ht="109.5" customHeight="1" spans="1:7">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" ht="54" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" ht="175.5" spans="1:3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" ht="67.5" spans="1:3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" ht="54" spans="1:4">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" ht="27" spans="1:4">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1727,10 +1819,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1743,150 +1835,174 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" ht="100" customHeight="1" spans="1:2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" ht="100" customHeight="1" spans="1:6">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" ht="100" customHeight="1" spans="1:1">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" ht="100" customHeight="1" spans="1:3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" ht="100" customHeight="1" spans="1:1">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" ht="100" customHeight="1" spans="1:1">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" ht="100" customHeight="1" spans="1:1">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" ht="100" customHeight="1" spans="1:2">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" ht="100" customHeight="1" spans="1:6">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" ht="100" customHeight="1" spans="1:1">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" ht="100" customHeight="1" spans="1:2">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" ht="100" customHeight="1" spans="1:4">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" ht="100" customHeight="1" spans="1:3">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" ht="67.5" spans="1:2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" ht="100" customHeight="1" spans="1:2">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" ht="135" spans="1:2">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" ht="27" spans="1:2">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1916,10 +2032,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit thingsboard rule engine test record
</commit_message>
<xml_diff>
--- a/reference/Q&A.xlsx
+++ b/reference/Q&A.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>备注1</t>
   </si>
@@ -683,6 +683,16 @@
       <t>：
 http://doc.oschina.net/grpc?t=60134</t>
     </r>
+  </si>
+  <si>
+    <t>kafka消息如何保证质量</t>
+  </si>
+  <si>
+    <t>Kafka的ack机制。
+当producer向leader发送数据时，可以通过request.required.acks参数来设置数据可靠性的级别：
+   1（默认）：这意味着producer在ISR中的leader已成功收到的数据并得到确认后发送下一条message。如果leader宕机了，则会丢失数据。
+   0：这意味着producer无需等待来自broker的确认而继续发送下一批消息。这种情况下数据传输效率最高，但是数据可靠性确是最低的。
+   -1：producer需要等待ISR中的所有follower都确认接收到数据后才算一次发送完成，可靠性最高。但是这样也不能保证数据不丢失，比如当ISR中只有leader时，这样就变成了acks=1的情况。</t>
   </si>
   <si>
     <t>kafka使用SASL认证配置方法</t>
@@ -2179,10 +2189,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A26" sqref="$A26:$XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -2463,6 +2473,14 @@
       </c>
       <c r="E25" s="9" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="26" ht="103.5" customHeight="1" spans="1:2">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2494,261 +2512,261 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" ht="100" customHeight="1" spans="1:2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" ht="100" customHeight="1" spans="1:6">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" ht="100" customHeight="1" spans="1:1">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" ht="100" customHeight="1" spans="1:3">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" ht="100" customHeight="1" spans="1:1">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" ht="100" customHeight="1" spans="1:1">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" ht="100" customHeight="1" spans="1:1">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" ht="100" customHeight="1" spans="1:2">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" ht="100" customHeight="1" spans="1:6">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" ht="100" customHeight="1" spans="1:1">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" ht="100" customHeight="1" spans="1:2">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" ht="100" customHeight="1" spans="1:4">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" ht="100" customHeight="1" spans="1:3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" ht="67.5" spans="1:2">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" ht="100" customHeight="1" spans="1:2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" ht="109.5" customHeight="1" spans="1:3">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" ht="27" spans="1:2">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" ht="108" spans="1:2">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" ht="121.5" spans="1:4">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" ht="40.5" spans="1:2">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" ht="88" customHeight="1" spans="1:3">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" ht="94.5" spans="1:3">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" ht="54" spans="1:2">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" ht="109.5" customHeight="1" spans="1:2">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" ht="27" spans="1:2">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2778,10 +2796,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>